<commit_message>
added results of power-law model
</commit_message>
<xml_diff>
--- a/code/all_keywords_Estimation.xlsx
+++ b/code/all_keywords_Estimation.xlsx
@@ -47,49 +47,49 @@
     <t xml:space="preserve">MLE-KS</t>
   </si>
   <si>
-    <t xml:space="preserve">2.076</t>
+    <t xml:space="preserve">2.393</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3069</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.019</t>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.033</t>
   </si>
   <si>
     <t xml:space="preserve">Bootstrapping</t>
   </si>
   <si>
-    <t xml:space="preserve">2.077</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.229</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.655</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2866.921</t>
-  </si>
-  <si>
-    <t xml:space="preserve">707.799</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
+    <t xml:space="preserve">2.414</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.672</t>
+  </si>
+  <si>
+    <t xml:space="preserve">173.172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.039</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.699</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated results power-law model for top 100 concepts
</commit_message>
<xml_diff>
--- a/code/all_keywords_Estimation.xlsx
+++ b/code/all_keywords_Estimation.xlsx
@@ -47,49 +47,49 @@
     <t xml:space="preserve">MLE-KS</t>
   </si>
   <si>
-    <t xml:space="preserve">2.393</t>
+    <t xml:space="preserve">2.337</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">188</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.033</t>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.055</t>
   </si>
   <si>
     <t xml:space="preserve">Bootstrapping</t>
   </si>
   <si>
-    <t xml:space="preserve">2.414</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.137</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.118</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5.672</t>
-  </si>
-  <si>
-    <t xml:space="preserve">173.172</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37.925</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.039</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.699</t>
+    <t xml:space="preserve">2.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.602</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.873</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87.513</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.628</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.438</t>
   </si>
 </sst>
 </file>

</xml_diff>